<commit_message>
revisi menu dan sub menu ukm
</commit_message>
<xml_diff>
--- a/Documen Aturusaha/daftar menu.xlsx
+++ b/Documen Aturusaha/daftar menu.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="217">
   <si>
     <t>menu</t>
   </si>
@@ -891,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -946,6 +946,45 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -958,36 +997,12 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1003,23 +1018,14 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1320,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:A122"/>
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1348,7 +1354,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="40" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1359,28 +1365,28 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="63"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="5" t="s">
         <v>190</v>
       </c>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="63"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="63"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="63"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1389,7 +1395,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="63"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1406,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="63"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1411,7 +1417,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="53"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1422,7 +1428,7 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1433,7 +1439,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="63"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1448,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="63"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1451,7 +1457,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="63"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
@@ -1461,7 +1467,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="53"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
@@ -1473,7 +1479,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="40" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1487,7 +1493,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="63"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1496,7 +1502,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="63"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1506,7 +1512,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="63"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1516,7 +1522,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="53"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
@@ -1528,7 +1534,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="52" t="s">
+      <c r="A20" s="40" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1542,7 +1548,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="53"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="9" t="s">
         <v>191</v>
       </c>
@@ -1568,7 +1574,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="40" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1582,7 +1588,7 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="63"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="5" t="s">
         <v>39</v>
       </c>
@@ -1593,7 +1599,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="63"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="5" t="s">
         <v>41</v>
       </c>
@@ -1604,7 +1610,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="63"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="5" t="s">
         <v>43</v>
       </c>
@@ -1616,7 +1622,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="53"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="11" t="s">
         <v>45</v>
       </c>
@@ -1628,7 +1634,7 @@
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="40" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -1639,7 +1645,7 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="63"/>
+      <c r="A29" s="41"/>
       <c r="B29" t="s">
         <v>49</v>
       </c>
@@ -1648,14 +1654,14 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="63"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="53"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="11" t="s">
         <v>52</v>
       </c>
@@ -1664,7 +1670,7 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="43" t="s">
         <v>54</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -1673,21 +1679,21 @@
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="64"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="64"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="10" t="s">
         <v>57</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="64"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="10" t="s">
         <v>58</v>
       </c>
@@ -1696,7 +1702,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="64"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="10" t="s">
         <v>60</v>
       </c>
@@ -1705,7 +1711,7 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="64"/>
+      <c r="A37" s="43"/>
       <c r="B37" t="s">
         <v>62</v>
       </c>
@@ -1714,7 +1720,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="64"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="10" t="s">
         <v>63</v>
       </c>
@@ -1723,7 +1729,7 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="64"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="10" t="s">
         <v>64</v>
       </c>
@@ -1732,21 +1738,21 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="64"/>
+      <c r="A40" s="43"/>
       <c r="B40" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="64"/>
+      <c r="A41" s="43"/>
       <c r="B41" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="52" t="s">
+      <c r="A42" s="40" t="s">
         <v>68</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1755,49 +1761,49 @@
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="63"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="63"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="63"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="5" t="s">
         <v>72</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="63"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="63"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="53"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="52" t="s">
+      <c r="A49" s="40" t="s">
         <v>76</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1808,7 +1814,7 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="63"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="5" t="s">
         <v>79</v>
       </c>
@@ -1817,7 +1823,7 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="63"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="5" t="s">
         <v>81</v>
       </c>
@@ -1826,7 +1832,7 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="63"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="5" t="s">
         <v>83</v>
       </c>
@@ -1835,7 +1841,7 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="63"/>
+      <c r="A53" s="41"/>
       <c r="B53" s="5" t="s">
         <v>85</v>
       </c>
@@ -1844,7 +1850,7 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="63"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="5" t="s">
         <v>87</v>
       </c>
@@ -1853,7 +1859,7 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="63"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="5" t="s">
         <v>90</v>
       </c>
@@ -1862,7 +1868,7 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="63"/>
+      <c r="A56" s="41"/>
       <c r="B56" s="5" t="s">
         <v>92</v>
       </c>
@@ -1871,7 +1877,7 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="63"/>
+      <c r="A57" s="41"/>
       <c r="B57" s="5" t="s">
         <v>94</v>
       </c>
@@ -1880,7 +1886,7 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="63"/>
+      <c r="A58" s="41"/>
       <c r="B58" s="5" t="s">
         <v>96</v>
       </c>
@@ -1889,21 +1895,21 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="63"/>
+      <c r="A59" s="41"/>
       <c r="B59" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C59" s="5"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="53"/>
+      <c r="A60" s="42"/>
       <c r="B60" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C60" s="5"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="52" t="s">
+      <c r="A61" s="40" t="s">
         <v>100</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1912,49 +1918,49 @@
       <c r="C61" s="5"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="63"/>
+      <c r="A62" s="41"/>
       <c r="B62" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C62" s="5"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="63"/>
+      <c r="A63" s="41"/>
       <c r="B63" s="17" t="s">
         <v>103</v>
       </c>
       <c r="C63" s="5"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="63"/>
+      <c r="A64" s="41"/>
       <c r="B64" s="17" t="s">
         <v>104</v>
       </c>
       <c r="C64" s="5"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="63"/>
+      <c r="A65" s="41"/>
       <c r="B65" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C65" s="5"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="63"/>
+      <c r="A66" s="41"/>
       <c r="B66" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="53"/>
+      <c r="A67" s="42"/>
       <c r="B67" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="52" t="s">
+      <c r="A68" s="40" t="s">
         <v>108</v>
       </c>
       <c r="B68" s="13" t="s">
@@ -1963,14 +1969,14 @@
       <c r="C68" s="14"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="63"/>
+      <c r="A69" s="41"/>
       <c r="B69" s="31" t="s">
         <v>110</v>
       </c>
       <c r="C69" s="5"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="63"/>
+      <c r="A70" s="41"/>
       <c r="B70" s="15" t="s">
         <v>111</v>
       </c>
@@ -1979,35 +1985,35 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="63"/>
+      <c r="A71" s="41"/>
       <c r="B71" s="16" t="s">
         <v>113</v>
       </c>
       <c r="C71" s="5"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="63"/>
+      <c r="A72" s="41"/>
       <c r="B72" s="16" t="s">
         <v>114</v>
       </c>
       <c r="C72" s="5"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="63"/>
+      <c r="A73" s="41"/>
       <c r="B73" s="16" t="s">
         <v>115</v>
       </c>
       <c r="C73" s="5"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="63"/>
+      <c r="A74" s="41"/>
       <c r="B74" s="16" t="s">
         <v>116</v>
       </c>
       <c r="C74" s="5"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="53"/>
+      <c r="A75" s="42"/>
       <c r="B75" s="15" t="s">
         <v>117</v>
       </c>
@@ -2016,7 +2022,7 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="52" t="s">
+      <c r="A76" s="40" t="s">
         <v>119</v>
       </c>
       <c r="B76" s="15" t="s">
@@ -2027,14 +2033,14 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="63"/>
+      <c r="A77" s="41"/>
       <c r="B77" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C77" s="5"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="63"/>
+      <c r="A78" s="41"/>
       <c r="B78" s="15" t="s">
         <v>123</v>
       </c>
@@ -2090,7 +2096,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" s="5" customFormat="1">
-      <c r="A84" s="49"/>
+      <c r="A84" s="52"/>
       <c r="B84" s="17" t="s">
         <v>134</v>
       </c>
@@ -2125,7 +2131,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" s="5" customFormat="1">
-      <c r="A88" s="59" t="s">
+      <c r="A88" s="46" t="s">
         <v>185</v>
       </c>
       <c r="B88" s="5" t="s">
@@ -2136,25 +2142,25 @@
       </c>
     </row>
     <row r="89" spans="1:3" s="5" customFormat="1">
-      <c r="A89" s="59"/>
+      <c r="A89" s="46"/>
       <c r="B89" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:3" s="5" customFormat="1">
-      <c r="A90" s="59"/>
+      <c r="A90" s="46"/>
       <c r="B90" s="5" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="91" spans="1:3" s="5" customFormat="1">
-      <c r="A91" s="59"/>
+      <c r="A91" s="46"/>
       <c r="B91" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="92" spans="1:3" s="5" customFormat="1">
-      <c r="A92" s="50" t="s">
+      <c r="A92" s="57" t="s">
         <v>141</v>
       </c>
       <c r="B92" s="19" t="s">
@@ -2165,7 +2171,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" s="5" customFormat="1">
-      <c r="A93" s="50"/>
+      <c r="A93" s="57"/>
       <c r="B93" s="19" t="s">
         <v>144</v>
       </c>
@@ -2174,7 +2180,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" s="5" customFormat="1">
-      <c r="A94" s="51"/>
+      <c r="A94" s="58"/>
       <c r="B94" s="19" t="s">
         <v>186</v>
       </c>
@@ -2225,7 +2231,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" s="5" customFormat="1">
-      <c r="A100" s="60" t="s">
+      <c r="A100" s="49" t="s">
         <v>151</v>
       </c>
       <c r="B100" s="21" t="s">
@@ -2236,7 +2242,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" s="5" customFormat="1">
-      <c r="A101" s="61"/>
+      <c r="A101" s="50"/>
       <c r="B101" s="21" t="s">
         <v>199</v>
       </c>
@@ -2245,7 +2251,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" s="5" customFormat="1">
-      <c r="A102" s="61"/>
+      <c r="A102" s="50"/>
       <c r="B102" s="21" t="s">
         <v>203</v>
       </c>
@@ -2254,7 +2260,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" s="5" customFormat="1">
-      <c r="A103" s="61"/>
+      <c r="A103" s="50"/>
       <c r="B103" s="21" t="s">
         <v>204</v>
       </c>
@@ -2263,7 +2269,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" s="5" customFormat="1">
-      <c r="A104" s="61"/>
+      <c r="A104" s="50"/>
       <c r="B104" s="37" t="s">
         <v>202</v>
       </c>
@@ -2272,7 +2278,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" s="5" customFormat="1">
-      <c r="A105" s="62"/>
+      <c r="A105" s="51"/>
       <c r="B105" s="22" t="s">
         <v>205</v>
       </c>
@@ -2329,7 +2335,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" s="23" customFormat="1">
-      <c r="A111" s="49"/>
+      <c r="A111" s="52"/>
       <c r="B111" s="20" t="s">
         <v>211</v>
       </c>
@@ -2338,7 +2344,7 @@
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="54" t="s">
+      <c r="A112" s="59" t="s">
         <v>161</v>
       </c>
       <c r="B112" s="24" t="s">
@@ -2349,7 +2355,7 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="55"/>
+      <c r="A113" s="60"/>
       <c r="B113" s="25" t="s">
         <v>212</v>
       </c>
@@ -2358,7 +2364,7 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="55"/>
+      <c r="A114" s="60"/>
       <c r="B114" s="25" t="s">
         <v>213</v>
       </c>
@@ -2367,7 +2373,7 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="55"/>
+      <c r="A115" s="60"/>
       <c r="B115" s="25" t="s">
         <v>165</v>
       </c>
@@ -2376,14 +2382,14 @@
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="56"/>
+      <c r="A116" s="61"/>
       <c r="B116" s="25" t="s">
         <v>167</v>
       </c>
       <c r="C116" s="26"/>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="57" t="s">
+      <c r="A117" s="62" t="s">
         <v>170</v>
       </c>
       <c r="B117" s="29" t="s">
@@ -2392,42 +2398,42 @@
       <c r="C117" s="5"/>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="58"/>
+      <c r="A118" s="63"/>
       <c r="B118" s="29" t="s">
         <v>216</v>
       </c>
       <c r="C118" s="5"/>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="58"/>
+      <c r="A119" s="63"/>
       <c r="B119" s="29" t="s">
         <v>55</v>
       </c>
       <c r="C119" s="5"/>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="58"/>
+      <c r="A120" s="63"/>
       <c r="B120" s="29" t="s">
         <v>56</v>
       </c>
       <c r="C120" s="5"/>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="58"/>
+      <c r="A121" s="63"/>
       <c r="B121" s="29" t="s">
         <v>57</v>
       </c>
       <c r="C121" s="5"/>
     </row>
     <row r="122" spans="1:3" ht="30">
-      <c r="A122" s="58"/>
+      <c r="A122" s="63"/>
       <c r="B122" s="39" t="s">
         <v>214</v>
       </c>
       <c r="C122" s="5"/>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="52" t="s">
+      <c r="A123" s="40" t="s">
         <v>168</v>
       </c>
       <c r="B123" s="38" t="s">
@@ -2436,14 +2442,14 @@
       <c r="C123" s="5"/>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="53"/>
+      <c r="A124" s="42"/>
       <c r="B124" s="5" t="s">
         <v>188</v>
       </c>
       <c r="C124" s="5"/>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="41" t="s">
+      <c r="A125" s="54" t="s">
         <v>169</v>
       </c>
       <c r="B125" s="32" t="s">
@@ -2454,7 +2460,7 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="42"/>
+      <c r="A126" s="55"/>
       <c r="B126" s="32" t="s">
         <v>173</v>
       </c>
@@ -2463,7 +2469,7 @@
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="42"/>
+      <c r="A127" s="55"/>
       <c r="B127" s="32" t="s">
         <v>85</v>
       </c>
@@ -2472,7 +2478,7 @@
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="42"/>
+      <c r="A128" s="55"/>
       <c r="B128" s="32" t="s">
         <v>89</v>
       </c>
@@ -2481,28 +2487,28 @@
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="42"/>
+      <c r="A129" s="55"/>
       <c r="B129" s="32" t="s">
         <v>176</v>
       </c>
       <c r="C129" s="5"/>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="42"/>
+      <c r="A130" s="55"/>
       <c r="B130" s="32" t="s">
         <v>96</v>
       </c>
       <c r="C130" s="5"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="43"/>
+      <c r="A131" s="56"/>
       <c r="B131" s="33" t="s">
         <v>177</v>
       </c>
       <c r="C131" s="5"/>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="44" t="s">
+      <c r="A132" s="64" t="s">
         <v>171</v>
       </c>
       <c r="B132" s="34" t="s">
@@ -2511,62 +2517,87 @@
       <c r="C132" s="5"/>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="45"/>
+      <c r="A133" s="65"/>
       <c r="B133" s="34" t="s">
         <v>178</v>
       </c>
       <c r="C133" s="5"/>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="46"/>
+      <c r="A134" s="65"/>
       <c r="B134" s="34" t="s">
         <v>179</v>
       </c>
       <c r="C134" s="5"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="40" t="s">
+      <c r="A135" s="66"/>
+      <c r="B135" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C135" s="5"/>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="B135" s="35" t="s">
+      <c r="B136" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="27" t="s">
+      <c r="C136" s="5"/>
+      <c r="D136" s="27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="40"/>
-      <c r="B136" s="35" t="s">
+    <row r="137" spans="1:4">
+      <c r="A137" s="53"/>
+      <c r="B137" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="C136" s="5"/>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="40"/>
-      <c r="B137" s="35" t="s">
+      <c r="C137" s="5"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="53"/>
+      <c r="B138" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="C137" s="5"/>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="40"/>
-      <c r="B138" s="35" t="s">
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="53"/>
+      <c r="B139" s="35" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="40"/>
-      <c r="B139" s="35" t="s">
+    <row r="140" spans="1:4">
+      <c r="A140" s="53"/>
+      <c r="B140" s="35" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="8"/>
+    <row r="144" spans="1:4">
+      <c r="A144" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A125:A131"/>
+    <mergeCell ref="A106:A111"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A112:A116"/>
+    <mergeCell ref="A117:A122"/>
+    <mergeCell ref="A132:A135"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="A95:A99"/>
+    <mergeCell ref="A100:A105"/>
+    <mergeCell ref="A79:A84"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A28:A31"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A32:A41"/>
@@ -2574,24 +2605,6 @@
     <mergeCell ref="A49:A60"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="A95:A99"/>
-    <mergeCell ref="A100:A105"/>
-    <mergeCell ref="A79:A84"/>
-    <mergeCell ref="A135:A139"/>
-    <mergeCell ref="A125:A131"/>
-    <mergeCell ref="A132:A134"/>
-    <mergeCell ref="A106:A111"/>
-    <mergeCell ref="A92:A94"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A112:A116"/>
-    <mergeCell ref="A117:A122"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>